<commit_message>
Added online Q-Q stuff
</commit_message>
<xml_diff>
--- a/LinearRegressionQQ.xlsx
+++ b/LinearRegressionQQ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{5927B0A6-B592-4CFD-9945-E6E73E578F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{81C4EB93-9A07-473C-B3F6-C097F26791AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -1152,6 +1152,61 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Q-Q Plot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1182,7 +1237,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -2789,15 +2856,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>487680</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:rowOff>163830</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2820,6 +2887,94 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>448503</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>149055</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="A graph with orange dots&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BFC454C-0D5C-C6CE-7ADD-2BECB0A7EA36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6774180" y="6934200"/>
+          <a:ext cx="5934903" cy="3334215"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>508211</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>166037</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="A close-up of a number&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E0021DF-111A-CA0D-63EB-10B5105042D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="327660" y="10469880"/>
+          <a:ext cx="10612331" cy="2162477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3029,8 +3184,8 @@
   </sheetPr>
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Small diff between Excel and Online
</commit_message>
<xml_diff>
--- a/LinearRegressionQQ.xlsx
+++ b/LinearRegressionQQ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{81C4EB93-9A07-473C-B3F6-C097F26791AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E15136-0AD6-4CCE-A38E-C230C240A5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -36,6 +36,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -100,8 +122,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -255,8 +277,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -278,10 +300,10 @@
   </cellStyles>
   <dxfs count="22">
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.000000"/>
+      <numFmt numFmtId="165" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1218,7 +1240,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Report!$F$32</c:f>
+              <c:f>Report!$F$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1253,7 +1275,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Report!$E$33:$E$43</c:f>
+              <c:f>Report!$E$37:$E$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1295,7 +1317,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Report!$F$33:$F$43</c:f>
+              <c:f>Report!$F$37:$F$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2977,6 +2999,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>296082</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>55863</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="A screenshot of a calculator&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1510963-9812-78C4-8346-AF597B4DF7FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8602980" y="685800"/>
+          <a:ext cx="5782482" cy="4429743"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2985,8 +3051,8 @@
   <autoFilter ref="A6:C17" xr:uid="{56545C43-D3C4-4189-86EB-EFBFD19DACF0}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{06653C2A-E279-47FE-80AE-04D30DF773BA}" name="VBAT" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{9E14BE7B-187F-4A96-B735-560413BD6B64}" name="VHA" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{23CADCB1-92D2-4A1A-A3A0-1F5B6770F8E6}" name="Residual" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{9E14BE7B-187F-4A96-B735-560413BD6B64}" name="VHA" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{23CADCB1-92D2-4A1A-A3A0-1F5B6770F8E6}" name="Residual" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3182,10 +3248,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3205,7 +3271,7 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>0.33100000000000002</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -3216,7 +3282,7 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>-1.7000000000000001E-2</v>
       </c>
     </row>
@@ -3341,7 +3407,7 @@
         <v>3.9982082700433796E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>4.1000000000000005</v>
       </c>
@@ -3352,7 +3418,7 @@
         <v>-3.9328955919875064E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -3361,7 +3427,7 @@
         <v>0.33133941522841298</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -3370,229 +3436,186 @@
         <v>-1.7581727399808678E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" cm="1">
+        <f t="array" ref="A22:B26">LINEST(Table1[VHA],Table1[VBAT],TRUE,TRUE)</f>
+        <v>0.33133941522841298</v>
+      </c>
+      <c r="B22">
+        <v>-1.7581727399808678E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3.3368636756318519E-3</v>
+      </c>
+      <c r="B23">
+        <v>1.2058965503647158E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.99908803747107588</v>
+      </c>
+      <c r="B24">
+        <v>3.4997321481402633E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9859.8265302055133</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.12076438889229747</v>
+      </c>
+      <c r="B26">
+        <v>1.1023312597853816E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
         <f>RSQ(Table1[VHA],Table1[VBAT])</f>
         <v>0.99908803747107611</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="34" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
+    <row r="35" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="6" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F36" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37">
         <v>-4.0362495554233657E-3</v>
       </c>
-      <c r="C33">
-        <f>_xlfn.RANK.AVG(B33,$B$33:$B$43,1)</f>
+      <c r="C37">
+        <f>_xlfn.RANK.AVG(B37,$B$37:$B$47,1)</f>
         <v>1</v>
       </c>
-      <c r="D33">
-        <f>(C33-0.5)/COUNT($C$33:$C$43)</f>
+      <c r="D37">
+        <f>(C37-0.5)/COUNT($C$37:$C$47)</f>
         <v>4.5454545454545456E-2</v>
       </c>
-      <c r="E33">
-        <f>_xlfn.NORM.S.INV(D33)</f>
+      <c r="E37">
+        <f>_xlfn.NORM.S.INV(D37)</f>
         <v>-1.6906216295848977</v>
       </c>
-      <c r="F33">
-        <f>STANDARDIZE(B33,AVERAGE($B$33:$B$43),_xlfn.STDEV.S($B$33:$B$43))</f>
+      <c r="F37">
+        <f>STANDARDIZE(B37,AVERAGE($B$37:$B$47),_xlfn.STDEV.S($B$37:$B$47))</f>
         <v>-1.4076921211757378</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38">
         <v>-3.9328955919875064E-3</v>
       </c>
-      <c r="C34">
-        <f t="shared" ref="C34:C43" si="0">_xlfn.RANK.AVG(B34,$B$33:$B$43,1)</f>
+      <c r="C38">
+        <f>_xlfn.RANK.AVG(B38,$B$37:$B$47,1)</f>
         <v>2</v>
       </c>
-      <c r="D34">
-        <f t="shared" ref="D34:D43" si="1">(C34-0.5)/COUNT($C$33:$C$43)</f>
+      <c r="D38">
+        <f>(C38-0.5)/COUNT($C$37:$C$47)</f>
         <v>0.13636363636363635</v>
       </c>
-      <c r="E34">
-        <f t="shared" ref="E34:E43" si="2">_xlfn.NORM.S.INV(D34)</f>
+      <c r="E38">
+        <f t="shared" ref="E38:E47" si="0">_xlfn.NORM.S.INV(D38)</f>
         <v>-1.096803562093513</v>
       </c>
-      <c r="F34">
-        <f t="shared" ref="F34:F43" si="3">STANDARDIZE(B34,AVERAGE($B$33:$B$43),_xlfn.STDEV.S($B$33:$B$43))</f>
+      <c r="F38">
+        <f>STANDARDIZE(B38,AVERAGE($B$37:$B$47),_xlfn.STDEV.S($B$37:$B$47))</f>
         <v>-1.3765805755825054</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39">
         <v>-3.5076409578738144E-3</v>
       </c>
-      <c r="C35">
+      <c r="C39">
+        <f>_xlfn.RANK.AVG(B39,$B$37:$B$47,1)</f>
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <f>(C39-0.5)/COUNT($C$37:$C$47)</f>
+        <v>0.22727272727272727</v>
+      </c>
+      <c r="E39">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="1"/>
-        <v>0.22727272727272727</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="2"/>
         <v>-0.74785859476330196</v>
       </c>
-      <c r="F35">
-        <f t="shared" si="3"/>
+      <c r="F39">
+        <f>STANDARDIZE(B39,AVERAGE($B$37:$B$47),_xlfn.STDEV.S($B$37:$B$47))</f>
         <v>-1.2485706909284717</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40">
         <v>-1.2650865637342523E-3</v>
       </c>
-      <c r="C36">
+      <c r="C40">
+        <f>_xlfn.RANK.AVG(B40,$B$37:$B$47,1)</f>
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <f>(C40-0.5)/COUNT($C$37:$C$47)</f>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="E40">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="1"/>
-        <v>0.31818181818181818</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="2"/>
         <v>-0.47278912099226744</v>
       </c>
-      <c r="F36">
-        <f t="shared" si="3"/>
+      <c r="F40">
+        <f>STANDARDIZE(B40,AVERAGE($B$37:$B$47),_xlfn.STDEV.S($B$37:$B$47))</f>
         <v>-0.57351836628418895</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41">
         <v>2.5298664930772929E-4</v>
       </c>
-      <c r="C37">
+      <c r="C41">
+        <f>_xlfn.RANK.AVG(B41,$B$37:$B$47,1)</f>
+        <v>5</v>
+      </c>
+      <c r="D41">
+        <f>(C41-0.5)/COUNT($C$37:$C$47)</f>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="E41">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="1"/>
-        <v>0.40909090909090912</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="2"/>
         <v>-0.22988411757923208</v>
       </c>
-      <c r="F37">
-        <f t="shared" si="3"/>
+      <c r="F41">
+        <f>STANDARDIZE(B41,AVERAGE($B$37:$B$47),_xlfn.STDEV.S($B$37:$B$47))</f>
         <v>-0.11654891478626947</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38">
-        <v>1.669091347787921E-3</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="3"/>
-        <v>0.30972603807413929</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39">
-        <v>2.7829323111738802E-3</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="1"/>
-        <v>0.59090909090909094</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="2"/>
-        <v>0.22988411757923222</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="3"/>
-        <v>0.64501374997207661</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40">
-        <v>3.0894385269835123E-3</v>
-      </c>
-      <c r="C40">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="D40">
-        <f t="shared" si="1"/>
-        <v>0.68181818181818177</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="2"/>
-        <v>0.47278912099226728</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="3"/>
-        <v>0.73727805983270855</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>3.236759414515733E-3</v>
-      </c>
-      <c r="C41">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="D41">
-        <f t="shared" si="1"/>
-        <v>0.77272727272727271</v>
-      </c>
-      <c r="E41">
-        <f t="shared" si="2"/>
-        <v>0.74785859476330196</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="3"/>
-        <v>0.78162450148744578</v>
       </c>
       <c r="H41" t="s">
         <v>16</v>
@@ -3601,25 +3624,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42">
-        <v>3.9982082700433796E-3</v>
+        <v>1.669091347787921E-3</v>
       </c>
       <c r="C42">
+        <f>_xlfn.RANK.AVG(B42,$B$37:$B$47,1)</f>
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <f>(C42-0.5)/COUNT($C$37:$C$47)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E42">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="1"/>
-        <v>0.86363636363636365</v>
-      </c>
-      <c r="E42">
-        <f t="shared" si="2"/>
-        <v>1.096803562093513</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <f t="shared" si="3"/>
-        <v>1.0108353609274408</v>
+        <f>STANDARDIZE(B42,AVERAGE($B$37:$B$47),_xlfn.STDEV.S($B$37:$B$47))</f>
+        <v>0.30972603807413929</v>
       </c>
       <c r="H42">
         <v>-2</v>
@@ -3628,25 +3651,25 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43">
-        <v>4.7542977964645239E-3</v>
+        <v>2.7829323111738802E-3</v>
       </c>
       <c r="C43">
+        <f>_xlfn.RANK.AVG(B43,$B$37:$B$47,1)</f>
+        <v>7</v>
+      </c>
+      <c r="D43">
+        <f>(C43-0.5)/COUNT($C$37:$C$47)</f>
+        <v>0.59090909090909094</v>
+      </c>
+      <c r="E43">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="1"/>
-        <v>0.95454545454545459</v>
-      </c>
-      <c r="E43">
-        <f t="shared" si="2"/>
-        <v>1.6906216295848984</v>
+        <v>0.22988411757923222</v>
       </c>
       <c r="F43">
-        <f t="shared" si="3"/>
-        <v>1.238432958463362</v>
+        <f>STANDARDIZE(B43,AVERAGE($B$37:$B$47),_xlfn.STDEV.S($B$37:$B$47))</f>
+        <v>0.64501374997207661</v>
       </c>
       <c r="H43">
         <v>2</v>
@@ -3655,9 +3678,93 @@
         <v>2</v>
       </c>
     </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>3.0894385269835123E-3</v>
+      </c>
+      <c r="C44">
+        <f>_xlfn.RANK.AVG(B44,$B$37:$B$47,1)</f>
+        <v>8</v>
+      </c>
+      <c r="D44">
+        <f>(C44-0.5)/COUNT($C$37:$C$47)</f>
+        <v>0.68181818181818177</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>0.47278912099226728</v>
+      </c>
+      <c r="F44">
+        <f>STANDARDIZE(B44,AVERAGE($B$37:$B$47),_xlfn.STDEV.S($B$37:$B$47))</f>
+        <v>0.73727805983270855</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>3.236759414515733E-3</v>
+      </c>
+      <c r="C45">
+        <f>_xlfn.RANK.AVG(B45,$B$37:$B$47,1)</f>
+        <v>9</v>
+      </c>
+      <c r="D45">
+        <f>(C45-0.5)/COUNT($C$37:$C$47)</f>
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>0.74785859476330196</v>
+      </c>
+      <c r="F45">
+        <f>STANDARDIZE(B45,AVERAGE($B$37:$B$47),_xlfn.STDEV.S($B$37:$B$47))</f>
+        <v>0.78162450148744578</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>3.9982082700433796E-3</v>
+      </c>
+      <c r="C46">
+        <f>_xlfn.RANK.AVG(B46,$B$37:$B$47,1)</f>
+        <v>10</v>
+      </c>
+      <c r="D46">
+        <f>(C46-0.5)/COUNT($C$37:$C$47)</f>
+        <v>0.86363636363636365</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>1.096803562093513</v>
+      </c>
+      <c r="F46">
+        <f>STANDARDIZE(B46,AVERAGE($B$37:$B$47),_xlfn.STDEV.S($B$37:$B$47))</f>
+        <v>1.0108353609274408</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>4.7542977964645239E-3</v>
+      </c>
+      <c r="C47">
+        <f>_xlfn.RANK.AVG(B47,$B$37:$B$47,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D47">
+        <f>(C47-0.5)/COUNT($C$37:$C$47)</f>
+        <v>0.95454545454545459</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>1.6906216295848984</v>
+      </c>
+      <c r="F47">
+        <f>STANDARDIZE(B47,AVERAGE($B$37:$B$47),_xlfn.STDEV.S($B$37:$B$47))</f>
+        <v>1.238432958463362</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B33:B43">
-    <sortCondition ref="B33:B43"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B37:B47">
+    <sortCondition ref="B37:B47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>